<commit_message>
Release v0.7.3. No commands changes, only on excel protocol documentation
</commit_message>
<xml_diff>
--- a/extras/Nicebots-Pluggie-I2C-Commands.xlsx
+++ b/extras/Nicebots-Pluggie-I2C-Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casanovg\source\Repos\GitHub\timonel\apps\timonel-twim-ss\lib\nb-twi-cmd\extras\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\casanovg\source\Repos\GitHub\nb-twi-cmd\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A1FABE-96D9-438B-A5FA-E6B994ABEB8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B814D01-BA56-4A1D-90A9-86D7A943A9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{E9ADF2F8-A332-4D3D-AE91-D80A529ABDA6}"/>
+    <workbookView xWindow="1830" yWindow="570" windowWidth="22080" windowHeight="13770" xr2:uid="{E9ADF2F8-A332-4D3D-AE91-D80A529ABDA6}"/>
   </bookViews>
   <sheets>
     <sheet name="NB Command Set" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NB Command Set'!$B$7:$B$135</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -294,10 +297,10 @@
 - 1 byte Bootloader minor version number.
 - 1 byte Optional features settings.
 - 1 byte Extended optional features settings.
+- 1 byte Bootloader start address (LSB).
 - 1 byte Bootloader start address (MSB).
-- 1 byte Bootloader start address (LSB).
+- 1 byte Application start addr on the trampoline (LSB).
 - 1 byte Application start addr on the trampoline (MSB).
-- 1 byte Application start addr on the trampoline (LSB).
 - 1 byte AVR Low fuse bits settings.
 - 1 byte Internal RC oscillator calibration value.
 </t>
@@ -376,9 +379,48 @@
           <t xml:space="preserve">
 Command:
 - 1 byte OpCode.
+- 1 byte Base Address LSB.
 - 1 byte Base Address MSB.
-- 1 byte Base Address LSB.
-- 1 byte Checksum ((uint8_t ) Sum of MSB and LSB of the page address).
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 1 byte Checksum ((uint8_t ) Sum of LSB and MSB of the page address).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*) NOTE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: Until at least Timonel version 1.6, the bootloader ignores the TX checksum to save flash space. Instead, it sums the LSB and MSB received from the I2C master and returns it as RX checksum. So, the responsibility of determining if Timonel has correctly received the address sent by the I2C master is handed over to the latter, which should verify the RX checksum.
 </t>
         </r>
       </text>
@@ -405,7 +447,7 @@
           <t xml:space="preserve">
 Reply:
 - 1 byte Command Ack (~Command).
-- 1 byte Checksum (Sum of MSB and LSB of the received page address).</t>
+- 1 byte Checksum (Sum of LSB and MSB of the received page address).</t>
         </r>
       </text>
     </comment>
@@ -536,8 +578,8 @@
           <t xml:space="preserve">
 Command:
 - 1 byte OpCode.
+- 1 byte Base Address LSB.
 - 1 byte Base Address MSB.
-- 1 byte Base Address LSB.
 - 1 byte Data Size Requested.
 </t>
         </r>
@@ -566,7 +608,7 @@
           <t>Reply:
 - 1 byte Command Ack (~Command).
 - N bytes Data (1 byte for each 8-bit value).
-- 1 byte Checksum ((uint8_t) Sum of all data sent + MSB and LSB of the address received in the request).
+- 1 byte Checksum ((uint8_t) Sum of all data sent + LSB and MSB of the address received in the request).
 If SLV_PACKET_SIZE = 32, this command is to be executed 256 times to dump an ATtiny85 full flash memory.</t>
         </r>
       </text>
@@ -652,10 +694,49 @@
           <t xml:space="preserve">
 Command:
 - 1 byte OpCode.
+- 1 byte EEPROM Address LSB.
 - 1 byte EEPROM Address MSB.
-- 1 byte EEPROM Address LSB.
 - 1 byte Data.
-- 1 byte Checksum ((uint8_t ) Sum of MSB, LSB of the EEPROM address and data byte).
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 1 byte Checksum ((uint8_t ) Sum of LSB, MSB of the EEPROM address and data byte).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*) NOTE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: Until at least Timonel version 1.6, the bootloader ignores the TX checksum to save flash space. Instead, it sums the address LSB, MSB and data byte received from the I2C master and returns it as RX checksum. So, the responsibility of determining if Timonel has correctly received the address and data sent by the I2C master is handed over to the latter, which should verify the RX checksum.
 </t>
         </r>
       </text>
@@ -682,7 +763,8 @@
           <t xml:space="preserve">
 Reply:
 - 1 byte Command Ack (~Command).
-- 1 byte Checksum ((uint8_t ) Sum of MSB, LSB of the EEPROM address and data byte received).</t>
+- 1 byte Checksum ((uint8_t ) Sum of EEPROM address LSB, MSB and the data byte received).
+</t>
         </r>
       </text>
     </comment>
@@ -708,9 +790,48 @@
           <t xml:space="preserve">
 Command:
 - 1 byte OpCode.
+- 1 byte EEPROM Address LSB.
 - 1 byte EEPROM Address MSB.
-- 1 byte EEPROM Address LSB.
-- 1 byte Checksum ((uint8_t ) Sum of MSB and LSB of the EEPROM address).
+- </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 1 byte Checksum ((uint8_t ) Sum of LSB and MSB of the EEPROM address).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(*) NOTE</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">: Until at least Timonel version 1.6, the bootloader ignores the TX checksum to save flash space. Instead, it sums the address LSB, MSB and data byte sent to the I2C master and returns it as RX checksum. So, the responsibility of determining if Timonel has correctly received the address and data sent by the I2C master is handed over to the latter, which should verify the RX checksum.
 </t>
         </r>
       </text>
@@ -735,10 +856,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Reply:
+          <t xml:space="preserve">Reply:
 - 1 byte Command Ack (~Command).
 - 1 byte Data (1 byte for each 8-bit value).
-- 1 byte Checksum ((uint8_t) Sum of data byte sent + MSB and LSB of the EEPROM address received in the request).</t>
+- 1 byte Checksum ((uint8_t ) Sum of EEPROM address LSB, MSB and the data byte sent to the I2C master).
+</t>
         </r>
       </text>
     </comment>
@@ -2772,21 +2894,9 @@
     <t>// https://github.com/casanovg/nb-twi-cmd/raw/master/extras/Nicebots-Pluggie-I2C-Commands.xlsx</t>
   </si>
   <si>
-    <t>0.7.0</t>
-  </si>
-  <si>
     <t>into the actual "nb-twi-cmd.h" file</t>
   </si>
   <si>
-    <t>#ifndef _NB_TWI_CMD_H_</t>
-  </si>
-  <si>
-    <t>#define _NB_TWI_CMD_H_</t>
-  </si>
-  <si>
-    <t>#endif  // _NB_TWI_CMD_H_</t>
-  </si>
-  <si>
     <t>READ DEVICE SIGNATURE AND FUSES</t>
   </si>
   <si>
@@ -2812,6 +2922,18 @@
   </si>
   <si>
     <t>3 + Data + Csum</t>
+  </si>
+  <si>
+    <t>0.7.3</t>
+  </si>
+  <si>
+    <t>#ifndef NB_TWI_CMD_H</t>
+  </si>
+  <si>
+    <t>#define NB_TWI_CMD_H</t>
+  </si>
+  <si>
+    <t>#endif  // NB_TWI_CMD_H</t>
   </si>
 </sst>
 </file>
@@ -4064,11 +4186,11 @@
         <v>1</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>490</v>
+        <v>500</v>
       </c>
       <c r="AF3" s="5"/>
       <c r="AG3" s="6">
-        <v>44003</v>
+        <v>44377</v>
       </c>
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
@@ -5042,7 +5164,7 @@
       </c>
       <c r="AA13" s="37"/>
       <c r="AB13" s="49" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="AC13" s="36"/>
       <c r="AD13" s="47" t="s">
@@ -5550,7 +5672,7 @@
       </c>
       <c r="AA17" s="37"/>
       <c r="AB17" s="49" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="AC17" s="36"/>
       <c r="AD17" s="47" t="s">
@@ -5677,11 +5799,11 @@
       </c>
       <c r="AA18" s="37"/>
       <c r="AB18" s="49" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="AC18" s="36"/>
       <c r="AD18" s="47" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="AE18" s="47" t="str">
         <f t="shared" si="9"/>
@@ -5689,7 +5811,7 @@
       </c>
       <c r="AF18" s="36"/>
       <c r="AG18" s="47" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="AH18" s="47" t="str">
         <f t="shared" si="10"/>
@@ -5697,7 +5819,7 @@
       </c>
       <c r="AI18" s="36"/>
       <c r="AJ18" s="37" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="AK18" s="37">
         <v>2</v>
@@ -5804,11 +5926,11 @@
       </c>
       <c r="AA19" s="37"/>
       <c r="AB19" s="49" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="AC19" s="36"/>
       <c r="AD19" s="47" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="AE19" s="47" t="str">
         <f t="shared" si="9"/>
@@ -5816,7 +5938,7 @@
       </c>
       <c r="AF19" s="36"/>
       <c r="AG19" s="47" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="AH19" s="47" t="str">
         <f t="shared" si="10"/>
@@ -22828,7 +22950,7 @@
       </c>
       <c r="D4" s="103"/>
       <c r="E4" s="105" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F4" s="103"/>
       <c r="G4" s="103"/>
@@ -22863,13 +22985,13 @@
     <row r="10" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B10" s="104" t="str">
         <f>CONCATENATE("// *  Version: ", 'NB Command Set'!AE3, "                                      *")</f>
-        <v>// *  Version: 0.7.0                                      *</v>
+        <v>// *  Version: 0.7.3                                      *</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B11" s="104" t="str">
         <f>CONCATENATE("// *  ",  TEXT('NB Command Set'!AG3, "yyyy-mm-dd"),  " gustavo.casanova@nicebots.com            *")</f>
-        <v>// *  2020-06-21 gustavo.casanova@nicebots.com            *</v>
+        <v>// *  2021-06-30 gustavo.casanova@nicebots.com            *</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
@@ -22882,12 +23004,12 @@
     </row>
     <row r="14" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B14" s="104" t="s">
-        <v>492</v>
+        <v>501</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B15" s="104" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="13.5" x14ac:dyDescent="0.25">
@@ -26492,7 +26614,7 @@
     </row>
     <row r="276" spans="2:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B276" s="104" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
     </row>
     <row r="277" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>